<commit_message>
mise à jour de la matrice d'implication
</commit_message>
<xml_diff>
--- a/matrice d'implication GL.xlsx
+++ b/matrice d'implication GL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D371C25-A65E-4555-B3FD-56477A559D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92079CF9-3877-4BD2-8D39-1E1E6C020FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>projet :</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>tâches</t>
   </si>
@@ -47,34 +44,100 @@
     <t>étudiants</t>
   </si>
   <si>
-    <t>nom 1</t>
-  </si>
-  <si>
-    <t>nom 2</t>
-  </si>
-  <si>
-    <t>nom 3</t>
-  </si>
-  <si>
-    <t>nom 4</t>
-  </si>
-  <si>
-    <t>nom 5</t>
-  </si>
-  <si>
-    <t>date:</t>
-  </si>
-  <si>
-    <t>version:</t>
-  </si>
-  <si>
     <t>REMARQUES:</t>
   </si>
   <si>
     <t>MATRICE D'IMPLICATION : PROJET GL</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Diagramme de classe</t>
+  </si>
+  <si>
+    <t>projet : Genie Logiciel</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">date : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>05/01/2023</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">version : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>Création du SeedData</t>
+  </si>
+  <si>
+    <t>Création des Modèles</t>
+  </si>
+  <si>
+    <t>Creation du contexte et de la base de donnée</t>
+  </si>
+  <si>
+    <t>Crud Cinema</t>
+  </si>
+  <si>
+    <t>Crud Cinema API</t>
+  </si>
+  <si>
+    <t>Crud Film</t>
+  </si>
+  <si>
+    <t>Crud Film API</t>
+  </si>
+  <si>
+    <t>Crud Seance</t>
+  </si>
+  <si>
+    <t>Crud Seance API</t>
+  </si>
+  <si>
+    <t>Crud Salle</t>
+  </si>
+  <si>
+    <t>Test des curl GET</t>
+  </si>
+  <si>
+    <t>Test des curl PUT</t>
+  </si>
+  <si>
+    <t>Test des curl POST</t>
+  </si>
+  <si>
+    <t>Test des curl DELETE</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport</t>
+  </si>
+  <si>
+    <t>Diagramme Relationnel</t>
+  </si>
+  <si>
+    <t>Rebecca Grenet</t>
+  </si>
+  <si>
+    <t>Roche Eléa</t>
   </si>
 </sst>
 </file>
@@ -122,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -359,34 +422,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -406,11 +441,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,34 +504,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,46 +525,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -791,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H42"/>
+  <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -802,476 +885,472 @@
     <col min="1" max="1" width="9.1796875" style="1"/>
     <col min="2" max="2" width="9.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="37.81640625" style="1" customWidth="1"/>
-    <col min="4" max="8" width="19" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="5" width="19" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-    </row>
-    <row r="4" spans="2:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="13" t="s">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="2:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="30"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="26" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="24"/>
+    </row>
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>3</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C7" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <f>1+B7</f>
         <v>2</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C8" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <f t="shared" ref="B9:B34" si="0">1+B8</f>
         <v>3</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C11" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C12" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="36">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C13" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="35">
+        <v>1</v>
+      </c>
+      <c r="E13" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C14" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="35">
+        <v>1</v>
+      </c>
+      <c r="E14" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C15" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="E15" s="36">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C16" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="36">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C17" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="E17" s="36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C18" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="36">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C19" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="35">
+        <v>0</v>
+      </c>
+      <c r="E19" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="35">
+        <v>1</v>
+      </c>
+      <c r="E20" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C21" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="35">
+        <v>1</v>
+      </c>
+      <c r="E21" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="35">
+        <v>0</v>
+      </c>
+      <c r="E22" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C24" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+    </row>
+    <row r="35" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="5"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B36" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B37" s="16"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B38" s="16"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B39" s="16"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B40" s="16"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B41" s="16"/>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="3"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="34"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" s="10"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="10"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="10"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="10"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="10"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B2:H3"/>
+  <mergeCells count="4">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modification du Crud dans le SeanceController et SalleController en fonction des modèles SeanceDTO et SalleDTO
</commit_message>
<xml_diff>
--- a/matrice d'implication GL.xlsx
+++ b/matrice d'implication GL.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92079CF9-3877-4BD2-8D39-1E1E6C020FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F8A1C0-E51D-45E8-9749-39B47009EA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -877,7 +877,7 @@
   <dimension ref="B1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>